<commit_message>
final update static metadata
</commit_message>
<xml_diff>
--- a/Metadata/Bern/Meta_Bern.xlsx
+++ b/Metadata/Bern/Meta_Bern.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\A_Noémie\Studium\GIUB\Logger_Network\Metadata\Bern\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrick/Desktop/Work/Network/Bern/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F52719C-D361-4DAB-B78E-F297A36582B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE6BAC39-827B-6940-8D65-9771C66D7661}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14856" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blatt 1 - metadata_gen_2" sheetId="1" r:id="rId1"/>
@@ -902,7 +902,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -2377,31 +2377,31 @@
   </sheetPr>
   <dimension ref="A1:Q85"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="E72" sqref="E72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="19.95" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.77734375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="39.77734375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="7.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="39.83203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="25.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.77734375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14.44140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.77734375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.83203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" style="1" customWidth="1"/>
     <col min="7" max="8" width="10.33203125" style="1" customWidth="1"/>
     <col min="9" max="9" width="5.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="14.109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="14.1640625" style="1" customWidth="1"/>
     <col min="11" max="11" width="21" style="1" customWidth="1"/>
     <col min="12" max="12" width="27.33203125" style="1" customWidth="1"/>
     <col min="13" max="13" width="18.33203125" style="1" customWidth="1"/>
-    <col min="14" max="15" width="9.77734375" style="1" customWidth="1"/>
-    <col min="16" max="17" width="5.44140625" style="1" customWidth="1"/>
+    <col min="14" max="15" width="9.83203125" style="1" customWidth="1"/>
+    <col min="16" max="17" width="5.5" style="1" customWidth="1"/>
     <col min="18" max="18" width="8.33203125" style="1" customWidth="1"/>
     <col min="19" max="16384" width="8.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="19.95" customHeight="1">
+    <row r="1" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2454,7 +2454,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="11" customFormat="1" ht="20.25" customHeight="1">
+    <row r="2" spans="1:17" s="11" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -2503,7 +2503,7 @@
       </c>
       <c r="Q2" s="10"/>
     </row>
-    <row r="3" spans="1:17" s="11" customFormat="1" ht="20.25" customHeight="1">
+    <row r="3" spans="1:17" s="11" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="12">
         <v>2</v>
       </c>
@@ -2552,56 +2552,56 @@
       </c>
       <c r="Q3" s="17"/>
     </row>
-    <row r="4" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
-      <c r="A4" s="18">
+    <row r="4" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="27">
         <v>7</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="D4" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="21">
+      <c r="E4" s="30">
         <v>46.944789999999998</v>
       </c>
-      <c r="F4" s="21">
+      <c r="F4" s="30">
         <v>7.42713</v>
       </c>
-      <c r="G4" s="22">
+      <c r="G4" s="31">
         <v>2599124.4</v>
       </c>
-      <c r="H4" s="22">
+      <c r="H4" s="31">
         <v>1199300.1000000001</v>
       </c>
-      <c r="I4" s="22">
+      <c r="I4" s="31">
         <v>528.6</v>
       </c>
-      <c r="J4" s="20" t="s">
+      <c r="J4" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="K4" s="20" t="s">
+      <c r="K4" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="L4" s="20" t="s">
+      <c r="L4" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="M4" s="20" t="s">
+      <c r="M4" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="N4" s="20" t="s">
+      <c r="N4" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="O4" s="23"/>
-      <c r="P4" s="21">
-        <v>1</v>
-      </c>
-      <c r="Q4" s="23"/>
-    </row>
-    <row r="5" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+      <c r="O4" s="32"/>
+      <c r="P4" s="30">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="32"/>
+    </row>
+    <row r="5" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="18">
         <v>8</v>
       </c>
@@ -2650,7 +2650,7 @@
       </c>
       <c r="Q5" s="23"/>
     </row>
-    <row r="6" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+    <row r="6" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="18">
         <v>9</v>
       </c>
@@ -2699,7 +2699,7 @@
       </c>
       <c r="Q6" s="23"/>
     </row>
-    <row r="7" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+    <row r="7" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="18">
         <v>10</v>
       </c>
@@ -2748,7 +2748,7 @@
       </c>
       <c r="Q7" s="23"/>
     </row>
-    <row r="8" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+    <row r="8" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="18">
         <v>13</v>
       </c>
@@ -2797,7 +2797,7 @@
       </c>
       <c r="Q8" s="23"/>
     </row>
-    <row r="9" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+    <row r="9" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="18">
         <v>14</v>
       </c>
@@ -2846,7 +2846,7 @@
       </c>
       <c r="Q9" s="23"/>
     </row>
-    <row r="10" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+    <row r="10" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="18">
         <v>16</v>
       </c>
@@ -2895,7 +2895,7 @@
       </c>
       <c r="Q10" s="23"/>
     </row>
-    <row r="11" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+    <row r="11" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="18">
         <v>17</v>
       </c>
@@ -2944,7 +2944,7 @@
       </c>
       <c r="Q11" s="23"/>
     </row>
-    <row r="12" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+    <row r="12" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="18">
         <v>19</v>
       </c>
@@ -2993,56 +2993,56 @@
       </c>
       <c r="Q12" s="23"/>
     </row>
-    <row r="13" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
-      <c r="A13" s="18">
+    <row r="13" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="27">
         <v>21</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="C13" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="D13" s="20" t="s">
+      <c r="D13" s="29" t="s">
         <v>261</v>
       </c>
-      <c r="E13" s="21">
+      <c r="E13" s="30">
         <v>46.939639999999997</v>
       </c>
-      <c r="F13" s="21">
+      <c r="F13" s="30">
         <v>7.4416599999999997</v>
       </c>
-      <c r="G13" s="22">
+      <c r="G13" s="31">
         <v>2600230.5</v>
       </c>
-      <c r="H13" s="22">
+      <c r="H13" s="31">
         <v>1198727.8999999999</v>
       </c>
-      <c r="I13" s="22">
+      <c r="I13" s="31">
         <v>502.9</v>
       </c>
-      <c r="J13" s="20" t="s">
+      <c r="J13" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="K13" s="20" t="s">
+      <c r="K13" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="L13" s="20" t="s">
+      <c r="L13" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="M13" s="20" t="s">
+      <c r="M13" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="N13" s="20" t="s">
+      <c r="N13" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="O13" s="23"/>
-      <c r="P13" s="21">
-        <v>1</v>
-      </c>
-      <c r="Q13" s="23"/>
-    </row>
-    <row r="14" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+      <c r="O13" s="32"/>
+      <c r="P13" s="30">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="32"/>
+    </row>
+    <row r="14" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="18">
         <v>22</v>
       </c>
@@ -3091,7 +3091,7 @@
       </c>
       <c r="Q14" s="23"/>
     </row>
-    <row r="15" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+    <row r="15" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="18">
         <v>23</v>
       </c>
@@ -3140,7 +3140,7 @@
       </c>
       <c r="Q15" s="23"/>
     </row>
-    <row r="16" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+    <row r="16" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="18">
         <v>25</v>
       </c>
@@ -3189,7 +3189,7 @@
       </c>
       <c r="Q16" s="23"/>
     </row>
-    <row r="17" spans="1:17" s="45" customFormat="1" ht="19.95" customHeight="1">
+    <row r="17" spans="1:17" s="45" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="39">
         <v>26</v>
       </c>
@@ -3238,7 +3238,7 @@
       </c>
       <c r="Q17" s="44"/>
     </row>
-    <row r="18" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+    <row r="18" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="18">
         <v>28</v>
       </c>
@@ -3287,7 +3287,7 @@
       </c>
       <c r="Q18" s="23"/>
     </row>
-    <row r="19" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+    <row r="19" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="18">
         <v>30</v>
       </c>
@@ -3336,7 +3336,7 @@
       </c>
       <c r="Q19" s="23"/>
     </row>
-    <row r="20" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+    <row r="20" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="18">
         <v>31</v>
       </c>
@@ -3385,7 +3385,7 @@
       </c>
       <c r="Q20" s="23"/>
     </row>
-    <row r="21" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+    <row r="21" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="18">
         <v>32</v>
       </c>
@@ -3434,54 +3434,54 @@
       </c>
       <c r="Q21" s="23"/>
     </row>
-    <row r="22" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
-      <c r="A22" s="18">
+    <row r="22" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="27">
         <v>33</v>
       </c>
-      <c r="B22" s="19" t="s">
+      <c r="B22" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="C22" s="20" t="s">
+      <c r="C22" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="D22" s="20" t="s">
+      <c r="D22" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="E22" s="21">
+      <c r="E22" s="30">
         <v>46.937980000000003</v>
       </c>
-      <c r="F22" s="21">
+      <c r="F22" s="30">
         <v>7.4565599999999996</v>
       </c>
-      <c r="G22" s="22">
+      <c r="G22" s="31">
         <v>2601365.1</v>
       </c>
-      <c r="H22" s="22">
+      <c r="H22" s="31">
         <v>1198543.6000000001</v>
       </c>
-      <c r="I22" s="22">
+      <c r="I22" s="31">
         <v>535.20000000000005</v>
       </c>
-      <c r="J22" s="20" t="s">
+      <c r="J22" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="K22" s="20" t="s">
+      <c r="K22" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="L22" s="20" t="s">
+      <c r="L22" s="29" t="s">
         <v>100</v>
       </c>
-      <c r="M22" s="20" t="s">
+      <c r="M22" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="N22" s="23"/>
-      <c r="O22" s="23"/>
-      <c r="P22" s="21">
-        <v>1</v>
-      </c>
-      <c r="Q22" s="23"/>
-    </row>
-    <row r="23" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+      <c r="N22" s="32"/>
+      <c r="O22" s="32"/>
+      <c r="P22" s="30">
+        <v>1</v>
+      </c>
+      <c r="Q22" s="32"/>
+    </row>
+    <row r="23" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="18">
         <v>34</v>
       </c>
@@ -3530,7 +3530,7 @@
       </c>
       <c r="Q23" s="23"/>
     </row>
-    <row r="24" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+    <row r="24" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="18">
         <v>36</v>
       </c>
@@ -3579,7 +3579,7 @@
       </c>
       <c r="Q24" s="23"/>
     </row>
-    <row r="25" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+    <row r="25" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="18">
         <v>37</v>
       </c>
@@ -3628,7 +3628,7 @@
       </c>
       <c r="Q25" s="23"/>
     </row>
-    <row r="26" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+    <row r="26" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="18">
         <v>38</v>
       </c>
@@ -3677,7 +3677,7 @@
       </c>
       <c r="Q26" s="23"/>
     </row>
-    <row r="27" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+    <row r="27" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="18">
         <v>39</v>
       </c>
@@ -3726,7 +3726,7 @@
       </c>
       <c r="Q27" s="23"/>
     </row>
-    <row r="28" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+    <row r="28" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="18">
         <v>41</v>
       </c>
@@ -3775,7 +3775,7 @@
       </c>
       <c r="Q28" s="23"/>
     </row>
-    <row r="29" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+    <row r="29" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="18">
         <v>42</v>
       </c>
@@ -3824,7 +3824,7 @@
       </c>
       <c r="Q29" s="23"/>
     </row>
-    <row r="30" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+    <row r="30" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="18">
         <v>45</v>
       </c>
@@ -3873,7 +3873,7 @@
       </c>
       <c r="Q30" s="23"/>
     </row>
-    <row r="31" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+    <row r="31" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="18">
         <v>48</v>
       </c>
@@ -3922,7 +3922,7 @@
       </c>
       <c r="Q31" s="23"/>
     </row>
-    <row r="32" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+    <row r="32" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="18">
         <v>51</v>
       </c>
@@ -3971,7 +3971,7 @@
       </c>
       <c r="Q32" s="23"/>
     </row>
-    <row r="33" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+    <row r="33" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="18">
         <v>52</v>
       </c>
@@ -4020,7 +4020,7 @@
       </c>
       <c r="Q33" s="23"/>
     </row>
-    <row r="34" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+    <row r="34" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="18">
         <v>53</v>
       </c>
@@ -4069,7 +4069,7 @@
       </c>
       <c r="Q34" s="23"/>
     </row>
-    <row r="35" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+    <row r="35" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="18">
         <v>55</v>
       </c>
@@ -4118,7 +4118,7 @@
       </c>
       <c r="Q35" s="23"/>
     </row>
-    <row r="36" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+    <row r="36" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="18">
         <v>57</v>
       </c>
@@ -4167,7 +4167,7 @@
       </c>
       <c r="Q36" s="23"/>
     </row>
-    <row r="37" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+    <row r="37" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="18">
         <v>58</v>
       </c>
@@ -4216,7 +4216,7 @@
       </c>
       <c r="Q37" s="23"/>
     </row>
-    <row r="38" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+    <row r="38" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="18">
         <v>59</v>
       </c>
@@ -4265,7 +4265,7 @@
       </c>
       <c r="Q38" s="23"/>
     </row>
-    <row r="39" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+    <row r="39" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="18">
         <v>61</v>
       </c>
@@ -4314,7 +4314,7 @@
       </c>
       <c r="Q39" s="23"/>
     </row>
-    <row r="40" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+    <row r="40" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="18">
         <v>62</v>
       </c>
@@ -4363,7 +4363,7 @@
       </c>
       <c r="Q40" s="23"/>
     </row>
-    <row r="41" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+    <row r="41" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="18">
         <v>65</v>
       </c>
@@ -4412,7 +4412,7 @@
       </c>
       <c r="Q41" s="23"/>
     </row>
-    <row r="42" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+    <row r="42" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="18">
         <v>69</v>
       </c>
@@ -4461,7 +4461,7 @@
       </c>
       <c r="Q42" s="23"/>
     </row>
-    <row r="43" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+    <row r="43" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="18">
         <v>70</v>
       </c>
@@ -4510,7 +4510,7 @@
       </c>
       <c r="Q43" s="23"/>
     </row>
-    <row r="44" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+    <row r="44" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="18">
         <v>71</v>
       </c>
@@ -4559,7 +4559,7 @@
       </c>
       <c r="Q44" s="23"/>
     </row>
-    <row r="45" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+    <row r="45" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="18">
         <v>73</v>
       </c>
@@ -4608,7 +4608,7 @@
       </c>
       <c r="Q45" s="23"/>
     </row>
-    <row r="46" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+    <row r="46" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="18">
         <v>76</v>
       </c>
@@ -4657,7 +4657,7 @@
       </c>
       <c r="Q46" s="23"/>
     </row>
-    <row r="47" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+    <row r="47" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="18">
         <v>78</v>
       </c>
@@ -4706,7 +4706,7 @@
       </c>
       <c r="Q47" s="23"/>
     </row>
-    <row r="48" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+    <row r="48" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="18">
         <v>79</v>
       </c>
@@ -4755,7 +4755,7 @@
       </c>
       <c r="Q48" s="23"/>
     </row>
-    <row r="49" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+    <row r="49" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="18">
         <v>80</v>
       </c>
@@ -4804,7 +4804,7 @@
       </c>
       <c r="Q49" s="23"/>
     </row>
-    <row r="50" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+    <row r="50" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="18">
         <v>82</v>
       </c>
@@ -4853,7 +4853,7 @@
       </c>
       <c r="Q50" s="23"/>
     </row>
-    <row r="51" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+    <row r="51" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="18">
         <v>83</v>
       </c>
@@ -4902,7 +4902,7 @@
       </c>
       <c r="Q51" s="23"/>
     </row>
-    <row r="52" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+    <row r="52" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="18">
         <v>86</v>
       </c>
@@ -4951,7 +4951,7 @@
       </c>
       <c r="Q52" s="23"/>
     </row>
-    <row r="53" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+    <row r="53" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="18">
         <v>87</v>
       </c>
@@ -5000,7 +5000,7 @@
       </c>
       <c r="Q53" s="23"/>
     </row>
-    <row r="54" spans="1:17" s="2" customFormat="1" ht="19.95" customHeight="1">
+    <row r="54" spans="1:17" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="27">
         <v>89</v>
       </c>
@@ -5049,7 +5049,7 @@
       </c>
       <c r="Q54" s="32"/>
     </row>
-    <row r="55" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+    <row r="55" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="18">
         <v>98</v>
       </c>
@@ -5098,7 +5098,7 @@
       </c>
       <c r="Q55" s="23"/>
     </row>
-    <row r="56" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+    <row r="56" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="18">
         <v>99</v>
       </c>
@@ -5147,7 +5147,7 @@
       </c>
       <c r="Q56" s="23"/>
     </row>
-    <row r="57" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+    <row r="57" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="18">
         <v>101</v>
       </c>
@@ -5196,7 +5196,7 @@
       </c>
       <c r="Q57" s="23"/>
     </row>
-    <row r="58" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+    <row r="58" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="18">
         <v>102</v>
       </c>
@@ -5245,7 +5245,7 @@
       </c>
       <c r="Q58" s="23"/>
     </row>
-    <row r="59" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+    <row r="59" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="18">
         <v>111</v>
       </c>
@@ -5294,7 +5294,7 @@
       </c>
       <c r="Q59" s="23"/>
     </row>
-    <row r="60" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+    <row r="60" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="18">
         <v>112</v>
       </c>
@@ -5343,7 +5343,7 @@
       </c>
       <c r="Q60" s="23"/>
     </row>
-    <row r="61" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+    <row r="61" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="18">
         <v>113</v>
       </c>
@@ -5392,7 +5392,7 @@
       </c>
       <c r="Q61" s="23"/>
     </row>
-    <row r="62" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+    <row r="62" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="18">
         <v>116</v>
       </c>
@@ -5441,7 +5441,7 @@
       </c>
       <c r="Q62" s="23"/>
     </row>
-    <row r="63" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+    <row r="63" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A63" s="18">
         <v>117</v>
       </c>
@@ -5490,7 +5490,7 @@
       </c>
       <c r="Q63" s="23"/>
     </row>
-    <row r="64" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+    <row r="64" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A64" s="18">
         <v>124</v>
       </c>
@@ -5539,7 +5539,7 @@
       </c>
       <c r="Q64" s="23"/>
     </row>
-    <row r="65" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+    <row r="65" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A65" s="18">
         <v>126</v>
       </c>
@@ -5588,7 +5588,7 @@
       </c>
       <c r="Q65" s="23"/>
     </row>
-    <row r="66" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+    <row r="66" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A66" s="18">
         <v>127</v>
       </c>
@@ -5637,7 +5637,7 @@
       </c>
       <c r="Q66" s="23"/>
     </row>
-    <row r="67" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+    <row r="67" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A67" s="18">
         <v>128</v>
       </c>
@@ -5674,56 +5674,56 @@
       <c r="P67" s="21"/>
       <c r="Q67" s="23"/>
     </row>
-    <row r="68" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
-      <c r="A68" s="18">
+    <row r="68" spans="1:17" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A68" s="27">
         <v>129</v>
       </c>
-      <c r="B68" s="19" t="s">
+      <c r="B68" s="28" t="s">
         <v>225</v>
       </c>
-      <c r="C68" s="20" t="s">
+      <c r="C68" s="29" t="s">
         <v>226</v>
       </c>
-      <c r="D68" s="20" t="s">
+      <c r="D68" s="29" t="s">
         <v>227</v>
       </c>
-      <c r="E68" s="21">
+      <c r="E68" s="30">
         <v>46.947339999999997</v>
       </c>
-      <c r="F68" s="21">
+      <c r="F68" s="30">
         <v>7.4363900000000003</v>
       </c>
-      <c r="G68" s="21">
+      <c r="G68" s="30">
         <v>2599829</v>
       </c>
-      <c r="H68" s="22">
+      <c r="H68" s="31">
         <v>1199583.8</v>
       </c>
-      <c r="I68" s="22">
+      <c r="I68" s="31">
         <v>540.6</v>
       </c>
-      <c r="J68" s="20" t="s">
+      <c r="J68" s="29" t="s">
         <v>206</v>
       </c>
-      <c r="K68" s="20" t="s">
+      <c r="K68" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="L68" s="20" t="s">
+      <c r="L68" s="29" t="s">
         <v>121</v>
       </c>
-      <c r="M68" s="20" t="s">
+      <c r="M68" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="N68" s="20" t="s">
+      <c r="N68" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="O68" s="23"/>
-      <c r="P68" s="21">
-        <v>1</v>
-      </c>
-      <c r="Q68" s="23"/>
-    </row>
-    <row r="69" spans="1:17" s="25" customFormat="1" ht="19.95" customHeight="1">
+      <c r="O68" s="32"/>
+      <c r="P68" s="30">
+        <v>1</v>
+      </c>
+      <c r="Q68" s="32"/>
+    </row>
+    <row r="69" spans="1:17" s="25" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A69" s="18">
         <v>134</v>
       </c>
@@ -5766,7 +5766,7 @@
       </c>
       <c r="Q69" s="23"/>
     </row>
-    <row r="70" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+    <row r="70" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A70" s="18">
         <v>135</v>
       </c>
@@ -5815,7 +5815,7 @@
       </c>
       <c r="Q70" s="23"/>
     </row>
-    <row r="71" spans="1:17" s="45" customFormat="1" ht="19.95" customHeight="1">
+    <row r="71" spans="1:17" s="45" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A71" s="39">
         <v>136</v>
       </c>
@@ -5864,7 +5864,7 @@
       </c>
       <c r="Q71" s="44"/>
     </row>
-    <row r="72" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+    <row r="72" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A72" s="18">
         <v>141</v>
       </c>
@@ -5913,7 +5913,7 @@
       </c>
       <c r="Q72" s="23"/>
     </row>
-    <row r="73" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+    <row r="73" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A73" s="18">
         <v>142</v>
       </c>
@@ -5962,7 +5962,7 @@
       </c>
       <c r="Q73" s="23"/>
     </row>
-    <row r="74" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+    <row r="74" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A74" s="18">
         <v>143</v>
       </c>
@@ -6011,7 +6011,7 @@
       </c>
       <c r="Q74" s="23"/>
     </row>
-    <row r="75" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+    <row r="75" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A75" s="18">
         <v>144</v>
       </c>
@@ -6060,7 +6060,7 @@
       </c>
       <c r="Q75" s="23"/>
     </row>
-    <row r="76" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+    <row r="76" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A76" s="18">
         <v>152</v>
       </c>
@@ -6109,7 +6109,7 @@
       </c>
       <c r="Q76" s="23"/>
     </row>
-    <row r="77" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+    <row r="77" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A77" s="18">
         <v>153</v>
       </c>
@@ -6158,7 +6158,7 @@
       </c>
       <c r="Q77" s="23"/>
     </row>
-    <row r="78" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+    <row r="78" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A78" s="18">
         <v>154</v>
       </c>
@@ -6207,7 +6207,7 @@
       </c>
       <c r="Q78" s="23"/>
     </row>
-    <row r="79" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+    <row r="79" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A79" s="18">
         <v>155</v>
       </c>
@@ -6256,7 +6256,7 @@
       </c>
       <c r="Q79" s="23"/>
     </row>
-    <row r="80" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+    <row r="80" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A80" s="18">
         <v>156</v>
       </c>
@@ -6305,7 +6305,7 @@
       </c>
       <c r="Q80" s="23"/>
     </row>
-    <row r="81" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+    <row r="81" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A81" s="18">
         <v>161</v>
       </c>
@@ -6354,7 +6354,7 @@
       </c>
       <c r="Q81" s="23"/>
     </row>
-    <row r="82" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+    <row r="82" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A82" s="18">
         <v>162</v>
       </c>
@@ -6403,7 +6403,7 @@
       </c>
       <c r="Q82" s="23"/>
     </row>
-    <row r="83" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+    <row r="83" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A83" s="26" t="s">
         <v>278</v>
       </c>
@@ -6452,7 +6452,7 @@
       </c>
       <c r="Q83" s="23"/>
     </row>
-    <row r="84" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+    <row r="84" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A84" s="26" t="s">
         <v>286</v>
       </c>
@@ -6501,7 +6501,7 @@
       </c>
       <c r="Q84" s="23"/>
     </row>
-    <row r="85" spans="1:17" s="11" customFormat="1" ht="19.95" customHeight="1">
+    <row r="85" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A85" s="26" t="s">
         <v>287</v>
       </c>

</xml_diff>